<commit_message>
end 15H, start 35H
</commit_message>
<xml_diff>
--- a/TInfenion_30H/IC_stock.xlsx
+++ b/TInfenion_30H/IC_stock.xlsx
@@ -1186,7 +1186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,6 +1238,53 @@
       <c r="I1" t="inlineStr">
         <is>
           <t>2023-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市远洋乾坤电子科技有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CY8C6247FTI-D52T</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CYPRESS/赛普拉斯</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
         </is>
       </c>
     </row>
@@ -1324,7 +1371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1376,6 +1423,53 @@
       <c r="I1" t="inlineStr">
         <is>
           <t>2023-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市美信美科技有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CY8C6245LQI-S3D72</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Cypress</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>5200</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2251,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2256,6 +2350,100 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>2023-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市昇源芯科技有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CY8C6247BZI-D34</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CYPRESS/实单来谈特价出售</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>3527</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市振东芯电子科技有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CY8C6247BZI-D34</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CYPRESS/实单来谈特价出售</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>3527</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
         </is>
       </c>
     </row>
@@ -3158,7 +3346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3257,6 +3445,100 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>2023-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市景宏锐科技有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>notSSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CY8C6247BZI-D44</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CYPRESS</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>5630</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市联煌电子有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CY8C6247BZI-D44</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CYPRESS</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>3790</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
         </is>
       </c>
     </row>

</xml_diff>